<commit_message>
menambah hari berdasarkan tanggal
</commit_message>
<xml_diff>
--- a/app/production/compatibility_model/dashboard/result/export/data_hasil/b450_2022-09-07.xlsx
+++ b/app/production/compatibility_model/dashboard/result/export/data_hasil/b450_2022-09-07.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>September 2022Production Schedule / Result For Assembly UP</t>
   </si>
@@ -42,6 +42,27 @@
   </si>
   <si>
     <t>Total Plan</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
   </si>
 </sst>
 </file>
@@ -510,7 +531,9 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -521,7 +544,9 @@
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -532,7 +557,9 @@
       <c r="A8" s="1">
         <v>3</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -543,7 +570,9 @@
       <c r="A9" s="1">
         <v>4</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -554,7 +583,9 @@
       <c r="A10" s="1">
         <v>5</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -565,7 +596,9 @@
       <c r="A11" s="1">
         <v>6</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -576,7 +609,9 @@
       <c r="A12" s="1">
         <v>7</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -587,7 +622,9 @@
       <c r="A13" s="1">
         <v>8</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -598,7 +635,9 @@
       <c r="A14" s="1">
         <v>9</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -609,7 +648,9 @@
       <c r="A15" s="1">
         <v>10</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -620,7 +661,9 @@
       <c r="A16" s="1">
         <v>11</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -631,7 +674,9 @@
       <c r="A17" s="1">
         <v>12</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -642,7 +687,9 @@
       <c r="A18" s="1">
         <v>13</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -653,7 +700,9 @@
       <c r="A19" s="1">
         <v>14</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -664,7 +713,9 @@
       <c r="A20" s="1">
         <v>15</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -675,7 +726,9 @@
       <c r="A21" s="1">
         <v>16</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -686,7 +739,9 @@
       <c r="A22" s="1">
         <v>17</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -697,7 +752,9 @@
       <c r="A23" s="1">
         <v>18</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -708,7 +765,9 @@
       <c r="A24" s="1">
         <v>19</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -719,7 +778,9 @@
       <c r="A25" s="1">
         <v>20</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -730,7 +791,9 @@
       <c r="A26" s="1">
         <v>21</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -741,7 +804,9 @@
       <c r="A27" s="1">
         <v>22</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -752,7 +817,9 @@
       <c r="A28" s="1">
         <v>23</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -763,7 +830,9 @@
       <c r="A29" s="1">
         <v>24</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -774,7 +843,9 @@
       <c r="A30" s="1">
         <v>25</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -785,7 +856,9 @@
       <c r="A31" s="1">
         <v>26</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -796,7 +869,9 @@
       <c r="A32" s="1">
         <v>27</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -807,7 +882,9 @@
       <c r="A33" s="1">
         <v>28</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -818,7 +895,9 @@
       <c r="A34" s="1">
         <v>29</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -829,7 +908,9 @@
       <c r="A35" s="1">
         <v>30</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>

</xml_diff>

<commit_message>
memperbarui data plan, karena ini untuk b450
</commit_message>
<xml_diff>
--- a/app/production/compatibility_model/dashboard/result/export/data_hasil/b450_2022-09-07.xlsx
+++ b/app/production/compatibility_model/dashboard/result/export/data_hasil/b450_2022-09-07.xlsx
@@ -29,7 +29,7 @@
     <t>Over Time</t>
   </si>
   <si>
-    <t>U200</t>
+    <t>B450</t>
   </si>
   <si>
     <t>Plan</t>
@@ -551,7 +551,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -611,7 +611,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -626,7 +626,7 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -641,7 +641,7 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -656,7 +656,7 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -716,7 +716,7 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -731,7 +731,7 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -746,7 +746,7 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -761,7 +761,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -836,7 +836,7 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -851,7 +851,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -866,7 +866,7 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -926,7 +926,7 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -956,7 +956,7 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>

</xml_diff>